<commit_message>
Updated Stanford Car dataset summary
Updated Stanford Car dataset summary
</commit_message>
<xml_diff>
--- a/Deep_Learning/Computer_Vision/Image_Classification/Stanford_Cars_Dataset/Stanford_Cars_Dataset_Classification_Model_Summary.xlsx
+++ b/Deep_Learning/Computer_Vision/Image_Classification/Stanford_Cars_Dataset/Stanford_Cars_Dataset_Classification_Model_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\User_Directories\Sync_With_NAS\Users\suresh\work\AIMLDL\GitHub_Repositories\Deep_Learning\Computer_Vision\Image_Classification\Stanford_Cars_Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BAE592-C616-4EAC-8A18-FA46F060F0D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB43F65-D824-4358-9FD4-479252FE3477}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
   <si>
     <t>Model</t>
   </si>
@@ -213,6 +213,15 @@
   </si>
   <si>
     <t>1) Early stopping at epoch 93</t>
+  </si>
+  <si>
+    <t>MA_9</t>
+  </si>
+  <si>
+    <t>1) Started with imgaug</t>
+  </si>
+  <si>
+    <t>rot:15, hf:T, wsr:0.15, hsr:0.15, sr:15, zr:0.15</t>
   </si>
 </sst>
 </file>
@@ -341,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -374,6 +383,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -383,7 +395,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -669,8 +681,8 @@
   <dimension ref="B1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,32 +710,32 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:19" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="12" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="12" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="12" t="s">
+      <c r="K2" s="14"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="2:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
@@ -965,7 +977,7 @@
       <c r="F7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="12" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="8" t="b">
@@ -1021,7 +1033,7 @@
       <c r="F8" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="11" t="b">
@@ -1077,7 +1089,7 @@
       <c r="F9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="11" t="b">
@@ -1133,7 +1145,7 @@
       <c r="F10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="12" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="11" t="b">
@@ -1173,25 +1185,45 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
+    <row r="11" spans="2:19" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>

</xml_diff>

<commit_message>
Added 1P55 and 1P56 equations
</commit_message>
<xml_diff>
--- a/Deep_Learning/Computer_Vision/Image_Classification/Stanford_Cars_Dataset/Stanford_Cars_Dataset_Classification_Model_Summary.xlsx
+++ b/Deep_Learning/Computer_Vision/Image_Classification/Stanford_Cars_Dataset/Stanford_Cars_Dataset_Classification_Model_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\User_Directories\Sync_With_NAS\Users\suresh\work\AIMLDL\GitHub_Repositories\Deep_Learning\Computer_Vision\Image_Classification\Stanford_Cars_Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2976500-6AC0-476F-AC4D-BF8133DFAF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA039EF-34A9-4C85-AC15-49F69D19BD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="115">
   <si>
     <t>Model</t>
   </si>
@@ -1271,6 +1271,12 @@
   <si>
     <t>1) Early stopping at epoch 88.
 2) Results with finalmodel.h5</t>
+  </si>
+  <si>
+    <t>InceptionResNetV2</t>
+  </si>
+  <si>
+    <t>(500, 500)</t>
   </si>
 </sst>
 </file>
@@ -1884,9 +1890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1896,7 +1902,7 @@
     <col min="3" max="3" width="11.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="1"/>
     <col min="9" max="9" width="12.21875" style="1" customWidth="1"/>
@@ -2519,32 +2525,50 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="20"/>
+      <c r="C13" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="L13" s="8">
         <v>159</v>
       </c>
       <c r="M13" s="8">
         <v>730</v>
       </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
     </row>
     <row r="14" spans="2:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
@@ -2637,6 +2661,7 @@
     <hyperlink ref="E11" location="Augmentation!B2" display="Aug_1" xr:uid="{ED982CAE-C36B-431F-BDDB-8097964C89A0}"/>
     <hyperlink ref="E12" location="Augmentation!B2" display="Aug_1" xr:uid="{9FA2B795-3521-427B-B7E9-F1CBD693A7BF}"/>
     <hyperlink ref="E14" location="Augmentation!B2" display="Aug_1" xr:uid="{96D72D16-A3BE-4F53-BCD5-AF3BE52BD1DF}"/>
+    <hyperlink ref="E13" location="Augmentation!B2" display="Aug_1" xr:uid="{C286F0CE-8086-41A0-8EBA-0DB7EE4D0C59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>